<commit_message>
oponentura 3. iterace ŠIP
</commit_message>
<xml_diff>
--- a/Výkazy/Michal Stanke.xlsx
+++ b/Výkazy/Michal Stanke.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Výkaz:</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Instalační manuál</t>
+  </si>
+  <si>
+    <t>kontrola a oponentura 3.iterace ŠIP</t>
   </si>
 </sst>
 </file>
@@ -510,11 +513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +545,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f>SUM(B7:B1002)</f>
-        <v>31</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -858,6 +861,14 @@
       </c>
       <c r="B44" s="8">
         <v>0.75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="8">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regenerace dokumentace 3. iterace
- s ohledem na opravu generování dokumentace
</commit_message>
<xml_diff>
--- a/Výkazy/Michal Stanke.xlsx
+++ b/Výkazy/Michal Stanke.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Výkaz:</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>kontrola a oponentura 3.iterace ŠIP</t>
+  </si>
+  <si>
+    <t>regenerace dokumentace 3. iterace</t>
   </si>
 </sst>
 </file>
@@ -513,11 +516,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+      <pane ySplit="6" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +548,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f>SUM(B7:B1002)</f>
-        <v>32.5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -869,6 +872,14 @@
       </c>
       <c r="B45" s="8">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="8">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
oponentura 4. iterace ŠIP
</commit_message>
<xml_diff>
--- a/Výkazy/Michal Stanke.xlsx
+++ b/Výkazy/Michal Stanke.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Výkaz:</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>aktualizace uživatelského manuálu</t>
+  </si>
+  <si>
+    <t>kontrola a oponentura 4.iterace ŠIP</t>
   </si>
 </sst>
 </file>
@@ -519,11 +522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +554,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f>SUM(B7:B1002)</f>
-        <v>34.5</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -899,6 +902,14 @@
       </c>
       <c r="B48" s="8">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aktualizace dokumentace - oprava testovacích scénářů
</commit_message>
<xml_diff>
--- a/Výkazy/Michal Stanke.xlsx
+++ b/Výkazy/Michal Stanke.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Výkaz:</t>
   </si>
@@ -154,7 +154,10 @@
     <t>aktualizace uživatelského manuálu</t>
   </si>
   <si>
-    <t>kontrola a oponentura 4.iterace ŠIP</t>
+    <t>kontrola a oponentura 4. iterace ŠIP</t>
+  </si>
+  <si>
+    <t>aktualizace dokumentace - oprava testovacích scénářů</t>
   </si>
 </sst>
 </file>
@@ -522,16 +525,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -554,7 +557,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f>SUM(B7:B1002)</f>
-        <v>35.5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -910,6 +913,14 @@
       </c>
       <c r="B49" s="8">
         <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="8">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>